<commit_message>
adding the ability to do shock on aggregated level
</commit_message>
<xml_diff>
--- a/kenya_sut/Database/Shock_shading.xlsx
+++ b/kenya_sut/Database/Shock_shading.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\negar\Documents\GitHub\CIVICS_Kenya\kenya_sut\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\kenya_sut\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C47C335-AB3A-4BF0-B3E0-DCD2193D0BF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5"/>
+    <workbookView xWindow="10065" yWindow="3480" windowWidth="28800" windowHeight="12855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Indeces" sheetId="8" r:id="rId5"/>
     <sheet name="main" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="219">
   <si>
     <t>level_row</t>
   </si>
@@ -685,12 +686,21 @@
   </si>
   <si>
     <t>#I think we have to increase the value added of the Skilled labors of high rainfall household production ( with multi practices of mulching, trenches, organic composting and shading tree we can have a general increase of 14% in the NPV)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Aggregated</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0;\-;\-"/>
@@ -1234,23 +1244,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1015625" style="1"/>
-    <col min="2" max="2" width="22.1015625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1015625" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1264,7 +1274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1281,21 +1291,21 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Percentage, Absolute"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1304,22 +1314,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1015625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1015625" style="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1327,7 +1337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1339,7 +1349,7 @@
         <v>29.099999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1351,16 +1361,16 @@
         <v>50.400000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
   </sheetData>
@@ -1368,7 +1378,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Indeces!$A$2:$A$72</xm:f>
           </x14:formula1>
@@ -1381,25 +1391,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1015625" style="1"/>
-    <col min="2" max="2" width="12.89453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.89453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1015625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1418,8 +1430,11 @@
       <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1442,8 +1457,11 @@
         <f>-main!C22</f>
         <v>-0.13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1466,8 +1484,11 @@
         <f>main!C23</f>
         <v>-3.6433199999999999E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H3" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1490,13 +1511,42 @@
         <f>main!C24</f>
         <v>-3.6433199999999999E-2</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>218</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Percentage, Absolute"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 B2:B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 B2:B5 C5" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Commodities,Activities"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1505,17 +1555,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>Indeces!$A$2:$A$72</xm:f>
           </x14:formula1>
           <xm:sqref>C3:C4 E2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
             <xm:f>Indeces!$B$2:$B$55</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E4 C2</xm:sqref>
+          <xm:sqref>E3:E5 C2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1524,24 +1574,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1015625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1015625" style="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1558,7 +1608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1578,24 +1628,24 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Commodities,Activities"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Percentage, Absolute"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1603,13 +1653,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000002000000}">
           <x14:formula1>
             <xm:f>Indeces!$C$2:$C$37</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000003000000}">
           <x14:formula1>
             <xm:f>Indeces!$B$2:$B$55</xm:f>
           </x14:formula1>
@@ -1622,21 +1672,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="56.89453125" customWidth="1"/>
-    <col min="3" max="3" width="47.1015625" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -1648,7 +1698,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1659,7 +1709,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1670,7 +1720,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1681,7 +1731,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1692,7 +1742,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1703,7 +1753,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1714,7 +1764,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1725,7 +1775,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1736,7 +1786,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1747,7 +1797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1758,7 +1808,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1769,7 +1819,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1780,7 +1830,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1791,7 +1841,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1806,7 +1856,7 @@
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1817,7 +1867,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1828,7 +1878,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1839,7 +1889,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1850,7 +1900,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1861,7 +1911,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1872,7 +1922,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1883,7 +1933,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1894,7 +1944,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1905,7 +1955,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1916,7 +1966,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1927,7 +1977,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1938,7 +1988,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1949,7 +1999,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1960,7 +2010,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1971,7 +2021,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1982,7 +2032,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1993,7 +2043,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2004,7 +2054,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2015,7 +2065,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2026,7 +2076,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2037,7 +2087,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2048,7 +2098,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2056,7 +2106,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2064,7 +2114,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2072,7 +2122,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2080,7 +2130,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2088,7 +2138,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2096,7 +2146,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2104,7 +2154,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -2112,7 +2162,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -2120,7 +2170,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2128,7 +2178,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2136,7 +2186,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2144,7 +2194,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2152,7 +2202,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2160,7 +2210,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2168,7 +2218,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2176,7 +2226,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -2184,7 +2234,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -2192,87 +2242,87 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -2283,29 +2333,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.15625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3125" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="186.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.62890625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1015625" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="186.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>178</v>
       </c>
@@ -2325,7 +2375,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>185</v>
       </c>
@@ -2341,7 +2391,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
       <c r="B3" s="14" t="s">
         <v>184</v>
@@ -2353,7 +2403,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="35"/>
       <c r="B4" s="12" t="s">
         <v>187</v>
@@ -2369,7 +2419,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="12" t="s">
         <v>188</v>
@@ -2381,7 +2431,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
       <c r="B6" s="12" t="s">
         <v>199</v>
@@ -2398,7 +2448,7 @@
       </c>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="B7" s="12" t="s">
         <v>193</v>
@@ -2410,7 +2460,7 @@
       </c>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="35"/>
       <c r="B8" s="12" t="s">
         <v>194</v>
@@ -2424,7 +2474,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="35"/>
       <c r="B9" s="12" t="s">
         <v>204</v>
@@ -2436,7 +2486,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="35"/>
       <c r="B10" s="12" t="s">
         <v>205</v>
@@ -2448,7 +2498,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
       <c r="B11" s="14" t="s">
         <v>186</v>
@@ -2462,7 +2512,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="14" t="s">
         <v>211</v>
@@ -2474,7 +2524,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>189</v>
       </c>
@@ -2488,7 +2538,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="34"/>
       <c r="B14" s="15" t="s">
         <v>200</v>
@@ -2498,7 +2548,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="15" t="s">
         <v>206</v>
@@ -2514,7 +2564,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="15" t="s">
         <v>207</v>
@@ -2530,7 +2580,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>180</v>
       </c>
@@ -2547,7 +2597,7 @@
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="33"/>
       <c r="B18" s="17" t="s">
         <v>191</v>
@@ -2562,7 +2612,7 @@
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="17" t="s">
         <v>192</v>
@@ -2575,7 +2625,7 @@
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>197</v>
       </c>
@@ -2594,7 +2644,7 @@
       </c>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
       <c r="B21" s="16" t="s">
         <v>175</v>
@@ -2611,7 +2661,7 @@
       </c>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="16" t="s">
         <v>196</v>
@@ -2625,7 +2675,7 @@
       </c>
       <c r="F22" s="16"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="36"/>
       <c r="B23" s="16" t="s">
         <v>212</v>
@@ -2640,7 +2690,7 @@
       </c>
       <c r="F23" s="16"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="36"/>
       <c r="B24" s="16" t="s">
         <v>213</v>
@@ -2655,11 +2705,11 @@
       </c>
       <c r="F24" s="16"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="20"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C29" s="20"/>
     </row>
   </sheetData>
@@ -2670,7 +2720,7 @@
     <mergeCell ref="A20:A24"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>